<commit_message>
Fixed data issue in .xlsx and .csv files
</commit_message>
<xml_diff>
--- a/2022/Goodreads 2022.xlsx
+++ b/2022/Goodreads 2022.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgillis/Desktop/Projects/books/2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgillis/Desktop/Projects/year-in-books/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A585B1B-1A0D-8248-A2AE-065730655D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86361E7F-4A18-CF4D-9D04-647A58D234F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15420" xr2:uid="{5EAF4BBB-85BB-3247-85D8-40D869713EBA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" xr2:uid="{5EAF4BBB-85BB-3247-85D8-40D869713EBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="88">
   <si>
     <t>Month Finished</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Dennis Lehane</t>
   </si>
   <si>
-    <t>Boston Noir</t>
-  </si>
-  <si>
     <t>Pastime</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>Thriller</t>
   </si>
   <si>
-    <t>Fiction</t>
-  </si>
-  <si>
     <t>James Stewart</t>
   </si>
   <si>
@@ -294,6 +288,18 @@
   </si>
   <si>
     <t>Nonfiction</t>
+  </si>
+  <si>
+    <t>Mini Math Crosswords</t>
+  </si>
+  <si>
+    <t>Brendan Sullivan</t>
+  </si>
+  <si>
+    <t>Puzzle</t>
+  </si>
+  <si>
+    <t>GR Rating (5 Star)</t>
   </si>
 </sst>
 </file>
@@ -337,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -345,6 +351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3238FA63-9DDE-7045-BBCC-D6A9DF0237F3}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -674,7 +681,7 @@
     <col min="6" max="6" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,8 +700,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -702,39 +712,45 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="F2" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>223</v>
+        <v>416</v>
       </c>
       <c r="F3" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -742,476 +758,548 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E4">
-        <v>416</v>
+        <v>525</v>
       </c>
       <c r="F4" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
       <c r="E5">
-        <v>525</v>
-      </c>
-      <c r="F5" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>512</v>
+      </c>
+      <c r="G5">
+        <v>3.82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>432</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>4.1500000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>18</v>
-      </c>
-      <c r="E6">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7">
-        <v>432</v>
+        <v>268</v>
       </c>
       <c r="F7" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>3.92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8">
-        <v>268</v>
+        <v>355</v>
       </c>
       <c r="F8" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
       </c>
       <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>448</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>4.16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9">
-        <v>355</v>
-      </c>
-      <c r="F9" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10">
-        <v>448</v>
+        <v>416</v>
       </c>
       <c r="F10" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11">
-        <v>416</v>
+        <v>480</v>
       </c>
       <c r="F11" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="E12">
-        <v>480</v>
+        <v>399</v>
       </c>
       <c r="F12" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>4.2699999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>272</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="D13" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13">
-        <v>399</v>
-      </c>
-      <c r="F13" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E14">
-        <v>272</v>
+        <v>419</v>
       </c>
       <c r="F14" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>3.61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E15">
-        <v>419</v>
+        <v>224</v>
       </c>
       <c r="F15" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>3.74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>211</v>
+      </c>
+      <c r="F16" s="2">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>3.96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
         <v>33</v>
       </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16">
-        <v>224</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>256</v>
+      </c>
+      <c r="F17" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="G17">
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17">
-        <v>211</v>
-      </c>
-      <c r="F17" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>36</v>
       </c>
       <c r="B18" t="s">
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E18">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="F18" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>3.97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>37</v>
       </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E19">
-        <v>250</v>
+        <v>372</v>
       </c>
       <c r="F19" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="G19">
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20">
+        <v>318</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>38</v>
-      </c>
-      <c r="C20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20">
-        <v>372</v>
-      </c>
-      <c r="F20" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>40</v>
       </c>
       <c r="B21" t="s">
         <v>41</v>
       </c>
       <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>282</v>
+      </c>
+      <c r="F21" s="2">
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
         <v>42</v>
       </c>
-      <c r="D21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21">
-        <v>318</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22">
+        <v>478</v>
+      </c>
+      <c r="F22" s="2">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>4.04</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
         <v>43</v>
       </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22">
-        <v>282</v>
-      </c>
-      <c r="F22" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>44</v>
       </c>
-      <c r="C23" t="s">
-        <v>23</v>
-      </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="E23">
-        <v>478</v>
+        <v>112</v>
       </c>
       <c r="F23" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
         <v>45</v>
       </c>
       <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <v>385</v>
+      </c>
+      <c r="F24" s="2">
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
         <v>46</v>
       </c>
-      <c r="D24" t="s">
-        <v>85</v>
-      </c>
-      <c r="E24">
-        <v>112</v>
-      </c>
-      <c r="F24" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25">
+        <v>311</v>
+      </c>
+      <c r="F25" s="2">
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
         <v>47</v>
       </c>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25">
-        <v>385</v>
-      </c>
-      <c r="F25" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" t="s">
-        <v>48</v>
-      </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E26">
-        <v>311</v>
+        <v>228</v>
       </c>
       <c r="F26" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
         <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E27">
-        <v>228</v>
+        <v>183</v>
       </c>
       <c r="F27" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -1219,416 +1307,476 @@
         <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E28">
-        <v>183</v>
+        <v>219</v>
       </c>
       <c r="F28" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" t="s">
         <v>52</v>
       </c>
-      <c r="B29" t="s">
-        <v>53</v>
-      </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E29">
-        <v>219</v>
+        <v>192</v>
       </c>
       <c r="F29" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30">
+        <v>221</v>
+      </c>
+      <c r="F30" s="2">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>4.1399999999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" t="s">
         <v>54</v>
       </c>
-      <c r="C30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30">
-        <v>192</v>
-      </c>
-      <c r="F30" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" t="s">
-        <v>55</v>
-      </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E31">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F31" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32">
+        <v>207</v>
+      </c>
+      <c r="F32" s="2">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>4.07</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" t="s">
         <v>56</v>
       </c>
-      <c r="C32" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32">
-        <v>219</v>
-      </c>
-      <c r="F32" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" t="s">
-        <v>57</v>
-      </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E33">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="F33" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>3.97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B34" t="s">
         <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E34">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="F34" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="G34">
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" t="s">
         <v>59</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35">
+        <v>205</v>
+      </c>
+      <c r="F35" s="2">
+        <v>4</v>
+      </c>
+      <c r="G35">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" t="s">
         <v>60</v>
       </c>
-      <c r="C35" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35">
-        <v>192</v>
-      </c>
-      <c r="F35" s="2">
+      <c r="C36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36">
+        <v>357</v>
+      </c>
+      <c r="F36" s="2">
+        <v>2</v>
+      </c>
+      <c r="G36">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37">
+        <v>476</v>
+      </c>
+      <c r="F37" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36">
-        <v>205</v>
-      </c>
-      <c r="F36" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="G37">
+        <v>4.5199999999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>62</v>
       </c>
-      <c r="C37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37">
-        <v>357</v>
-      </c>
-      <c r="F37" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>59</v>
-      </c>
       <c r="B38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D38" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E38">
-        <v>476</v>
+        <v>387</v>
       </c>
       <c r="F38" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>4.41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39">
+        <v>402</v>
+      </c>
+      <c r="F39" s="2">
+        <v>4</v>
+      </c>
+      <c r="G39">
+        <v>4.24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" t="s">
         <v>66</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40">
+        <v>480</v>
+      </c>
+      <c r="F40" s="2">
+        <v>5</v>
+      </c>
+      <c r="G40">
+        <v>4.03</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" t="s">
+        <v>81</v>
+      </c>
+      <c r="E41">
+        <v>304</v>
+      </c>
+      <c r="F41" s="2">
+        <v>2</v>
+      </c>
+      <c r="G41">
+        <v>4.0599999999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>69</v>
       </c>
-      <c r="D39" t="s">
-        <v>70</v>
-      </c>
-      <c r="E39">
-        <v>387</v>
-      </c>
-      <c r="F39" s="2">
+      <c r="B42" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42">
+        <v>208</v>
+      </c>
+      <c r="F42" s="2">
+        <v>4</v>
+      </c>
+      <c r="G42">
+        <v>3.92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43">
+        <v>406</v>
+      </c>
+      <c r="F43" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>64</v>
-      </c>
-      <c r="B40" t="s">
-        <v>67</v>
-      </c>
-      <c r="C40" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40">
-        <v>402</v>
-      </c>
-      <c r="F40" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>64</v>
-      </c>
-      <c r="B41" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41" t="s">
-        <v>23</v>
-      </c>
-      <c r="D41" t="s">
-        <v>15</v>
-      </c>
-      <c r="E41">
-        <v>480</v>
-      </c>
-      <c r="F41" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>64</v>
-      </c>
-      <c r="B42" t="s">
-        <v>73</v>
-      </c>
-      <c r="C42" t="s">
-        <v>82</v>
-      </c>
-      <c r="D42" t="s">
-        <v>83</v>
-      </c>
-      <c r="E42">
-        <v>304</v>
-      </c>
-      <c r="F42" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="G43">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" t="s">
         <v>74</v>
       </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43">
-        <v>208</v>
-      </c>
-      <c r="F43" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" t="s">
-        <v>75</v>
-      </c>
       <c r="C44" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D44" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E44">
-        <v>406</v>
+        <v>323</v>
       </c>
       <c r="F44" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>4.47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C45" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D45" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E45">
-        <v>323</v>
+        <v>407</v>
       </c>
       <c r="F45" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>4.38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B46" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46" t="s">
+        <v>82</v>
+      </c>
+      <c r="E46">
+        <v>342</v>
+      </c>
+      <c r="F46" s="2">
+        <v>3</v>
+      </c>
+      <c r="G46">
+        <v>4.03</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" t="s">
         <v>77</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" t="s">
         <v>82</v>
       </c>
-      <c r="D46" t="s">
-        <v>83</v>
-      </c>
-      <c r="E46">
-        <v>407</v>
-      </c>
-      <c r="F46" s="2">
+      <c r="E47">
+        <v>75</v>
+      </c>
+      <c r="F47" s="2">
+        <v>4</v>
+      </c>
+      <c r="G47">
+        <v>3.72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" t="s">
+        <v>86</v>
+      </c>
+      <c r="E48">
+        <v>82</v>
+      </c>
+      <c r="G48">
         <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>72</v>
-      </c>
-      <c r="B47" t="s">
-        <v>78</v>
-      </c>
-      <c r="C47" t="s">
-        <v>81</v>
-      </c>
-      <c r="D47" t="s">
-        <v>84</v>
-      </c>
-      <c r="E47">
-        <v>342</v>
-      </c>
-      <c r="F47" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>72</v>
-      </c>
-      <c r="B48" t="s">
-        <v>79</v>
-      </c>
-      <c r="C48" t="s">
-        <v>80</v>
-      </c>
-      <c r="D48" t="s">
-        <v>84</v>
-      </c>
-      <c r="E48">
-        <v>75</v>
-      </c>
-      <c r="F48" s="2">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created function that formats inline code.
</commit_message>
<xml_diff>
--- a/2022/Goodreads 2022.xlsx
+++ b/2022/Goodreads 2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgillis/Desktop/Projects/year-in-books/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86361E7F-4A18-CF4D-9D04-647A58D234F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C0C950-70FF-4443-9BFB-BD2DDB486DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" xr2:uid="{5EAF4BBB-85BB-3247-85D8-40D869713EBA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15480" xr2:uid="{5EAF4BBB-85BB-3247-85D8-40D869713EBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
fixing data to allow for NAs in ratings and standardizing column labels.
</commit_message>
<xml_diff>
--- a/2022/Goodreads 2022.xlsx
+++ b/2022/Goodreads 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgillis/Desktop/Projects/year-in-books/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C0C950-70FF-4443-9BFB-BD2DDB486DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B5D5A2-3434-6747-9431-E6D91282BF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15480" xr2:uid="{5EAF4BBB-85BB-3247-85D8-40D869713EBA}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Pages</t>
   </si>
   <si>
-    <t>Rating (5 Star)</t>
-  </si>
-  <si>
     <t>December</t>
   </si>
   <si>
@@ -299,7 +296,10 @@
     <t>Puzzle</t>
   </si>
   <si>
-    <t>GR Rating (5 Star)</t>
+    <t>My Rating</t>
+  </si>
+  <si>
+    <t>GR Rating</t>
   </si>
 </sst>
 </file>
@@ -343,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -351,7 +351,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3238FA63-9DDE-7045-BBCC-D6A9DF0237F3}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -698,24 +697,24 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>223</v>
@@ -729,16 +728,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>416</v>
@@ -752,16 +751,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
       </c>
       <c r="E4">
         <v>525</v>
@@ -775,16 +774,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
       </c>
       <c r="E5">
         <v>512</v>
@@ -795,16 +794,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6">
         <v>432</v>
@@ -818,16 +817,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>268</v>
@@ -841,16 +840,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8">
         <v>355</v>
@@ -864,16 +863,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9">
         <v>448</v>
@@ -887,16 +886,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10">
         <v>416</v>
@@ -910,16 +909,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11">
         <v>480</v>
@@ -933,16 +932,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E12">
         <v>399</v>
@@ -956,16 +955,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13">
         <v>272</v>
@@ -979,16 +978,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14">
         <v>419</v>
@@ -1002,16 +1001,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15">
         <v>224</v>
@@ -1025,16 +1024,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16">
         <v>211</v>
@@ -1048,16 +1047,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E17">
         <v>256</v>
@@ -1071,16 +1070,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18">
         <v>250</v>
@@ -1094,16 +1093,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
         <v>36</v>
       </c>
-      <c r="C19" t="s">
-        <v>37</v>
-      </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19">
         <v>372</v>
@@ -1117,16 +1116,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>39</v>
       </c>
-      <c r="C20" t="s">
-        <v>40</v>
-      </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <v>318</v>
@@ -1140,16 +1139,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E21">
         <v>282</v>
@@ -1163,16 +1162,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22">
         <v>478</v>
@@ -1186,16 +1185,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
         <v>43</v>
       </c>
-      <c r="C23" t="s">
-        <v>44</v>
-      </c>
       <c r="D23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E23">
         <v>112</v>
@@ -1209,16 +1208,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E24">
         <v>385</v>
@@ -1232,16 +1231,16 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E25">
         <v>311</v>
@@ -1255,16 +1254,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E26">
         <v>228</v>
@@ -1278,16 +1277,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
         <v>48</v>
       </c>
-      <c r="B27" t="s">
-        <v>49</v>
-      </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E27">
         <v>183</v>
@@ -1301,16 +1300,16 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" t="s">
         <v>50</v>
       </c>
-      <c r="B28" t="s">
-        <v>51</v>
-      </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E28">
         <v>219</v>
@@ -1324,16 +1323,16 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E29">
         <v>192</v>
@@ -1347,16 +1346,16 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E30">
         <v>221</v>
@@ -1370,16 +1369,16 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E31">
         <v>219</v>
@@ -1393,16 +1392,16 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E32">
         <v>207</v>
@@ -1416,16 +1415,16 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E33">
         <v>218</v>
@@ -1439,16 +1438,16 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" t="s">
         <v>57</v>
       </c>
-      <c r="B34" t="s">
-        <v>58</v>
-      </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E34">
         <v>192</v>
@@ -1462,16 +1461,16 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E35">
         <v>205</v>
@@ -1485,16 +1484,16 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" t="s">
         <v>60</v>
       </c>
-      <c r="C36" t="s">
-        <v>61</v>
-      </c>
       <c r="D36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E36">
         <v>357</v>
@@ -1508,16 +1507,16 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" t="s">
         <v>67</v>
-      </c>
-      <c r="D37" t="s">
-        <v>68</v>
       </c>
       <c r="E37">
         <v>476</v>
@@ -1531,16 +1530,16 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" t="s">
         <v>67</v>
-      </c>
-      <c r="D38" t="s">
-        <v>68</v>
       </c>
       <c r="E38">
         <v>387</v>
@@ -1554,16 +1553,16 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E39">
         <v>402</v>
@@ -1577,16 +1576,16 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E40">
         <v>480</v>
@@ -1600,16 +1599,16 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" t="s">
         <v>80</v>
-      </c>
-      <c r="D41" t="s">
-        <v>81</v>
       </c>
       <c r="E41">
         <v>304</v>
@@ -1623,16 +1622,16 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E42">
         <v>208</v>
@@ -1646,16 +1645,16 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C43" t="s">
+        <v>79</v>
+      </c>
+      <c r="D43" t="s">
         <v>80</v>
-      </c>
-      <c r="D43" t="s">
-        <v>81</v>
       </c>
       <c r="E43">
         <v>406</v>
@@ -1669,16 +1668,16 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C44" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" t="s">
         <v>80</v>
-      </c>
-      <c r="D44" t="s">
-        <v>81</v>
       </c>
       <c r="E44">
         <v>323</v>
@@ -1692,16 +1691,16 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D45" t="s">
         <v>80</v>
-      </c>
-      <c r="D45" t="s">
-        <v>81</v>
       </c>
       <c r="E45">
         <v>407</v>
@@ -1715,16 +1714,16 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B46" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E46">
         <v>342</v>
@@ -1738,16 +1737,16 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B47" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" t="s">
         <v>77</v>
       </c>
-      <c r="C47" t="s">
-        <v>78</v>
-      </c>
       <c r="D47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E47">
         <v>75</v>
@@ -1761,16 +1760,16 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B48" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" t="s">
         <v>84</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>85</v>
-      </c>
-      <c r="D48" t="s">
-        <v>86</v>
       </c>
       <c r="E48">
         <v>82</v>

</xml_diff>

<commit_message>
Moved docs to clean up repo.
</commit_message>
<xml_diff>
--- a/2022/Goodreads 2022.xlsx
+++ b/2022/Goodreads 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgillis/Desktop/Projects/year-in-books/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FD99ED-892C-5842-A2F8-61FFE5209CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E5D7D5-F810-3541-870B-E3B2B3B7336F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15480" xr2:uid="{5EAF4BBB-85BB-3247-85D8-40D869713EBA}"/>
   </bookViews>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3238FA63-9DDE-7045-BBCC-D6A9DF0237F3}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>